<commit_message>
getting rid of stuff
</commit_message>
<xml_diff>
--- a/Input_Data/week4/144L_2021_BactAbund.xlsx
+++ b/Input_Data/week4/144L_2021_BactAbund.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinealbers/Documents/144l_students_2021/Input_Data/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AA426-4900-B24C-B123-D8704D38B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F51BB19-03E2-4A4D-AC5B-07011462DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="-33700" yWindow="-5060" windowWidth="28580" windowHeight="17500" activeTab="3" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="FCM_Data" sheetId="2" r:id="rId2"/>
+    <sheet name="DAPI_Data" sheetId="3" r:id="rId3"/>
+    <sheet name="TOC_Data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="51">
   <si>
     <t>A</t>
   </si>
@@ -167,6 +169,27 @@
   </si>
   <si>
     <t>Kelp Exudate_Nitrate_Phosphate</t>
+  </si>
+  <si>
+    <t>Cells_mL</t>
+  </si>
+  <si>
+    <t>Cells_mL_Stdev</t>
+  </si>
+  <si>
+    <t>Mean_Biovolume_um3_cell</t>
+  </si>
+  <si>
+    <t>Biovolume_Stdev_um3_cell</t>
+  </si>
+  <si>
+    <t>Kelp_Exudate_Nitrate_Phosphate</t>
+  </si>
+  <si>
+    <t>Mean_uMC</t>
+  </si>
+  <si>
+    <t>Stdev_uMC</t>
   </si>
 </sst>
 </file>
@@ -527,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42:G61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5848,4 +5871,541 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C07682-43E0-9749-8711-A66C7C8B7855}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>660667</v>
+      </c>
+      <c r="D2">
+        <v>73217.755744736962</v>
+      </c>
+      <c r="E2">
+        <v>4.556209250166493E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.0548048518688944E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>919405.58319999999</v>
+      </c>
+      <c r="D3">
+        <v>363326.27392113575</v>
+      </c>
+      <c r="E3">
+        <v>5.0803531793108703E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.1000369174713136E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1133869.7239999999</v>
+      </c>
+      <c r="D4">
+        <v>99930.050143482484</v>
+      </c>
+      <c r="E4">
+        <v>4.0932122992205985E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.684495054588826E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>663088.10880000005</v>
+      </c>
+      <c r="D5">
+        <v>113546.26705004732</v>
+      </c>
+      <c r="E5">
+        <v>3.8714986197324441E-2</v>
+      </c>
+      <c r="F5">
+        <v>5.4464852650337146E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1043597.8280000003</v>
+      </c>
+      <c r="D6">
+        <v>181810.6237172893</v>
+      </c>
+      <c r="E6">
+        <v>6.8116291585186811E-2</v>
+      </c>
+      <c r="F6">
+        <v>1.3492316711132726E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1115268.2424000003</v>
+      </c>
+      <c r="D7">
+        <v>149497.94850320072</v>
+      </c>
+      <c r="E7">
+        <v>3.2720249084495917E-2</v>
+      </c>
+      <c r="F7">
+        <v>9.6971343755849169E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>672115.29839999997</v>
+      </c>
+      <c r="D8">
+        <v>71870.484141861118</v>
+      </c>
+      <c r="E8">
+        <v>3.6309706278979906E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.0124924763695301E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1226603.5808000001</v>
+      </c>
+      <c r="D9">
+        <v>153931.80801620887</v>
+      </c>
+      <c r="E9">
+        <v>0.10237022179025781</v>
+      </c>
+      <c r="F9">
+        <v>1.4780122705744487E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1391554.9543999997</v>
+      </c>
+      <c r="D10">
+        <v>81241.073296844464</v>
+      </c>
+      <c r="E10">
+        <v>6.1333789954676352E-2</v>
+      </c>
+      <c r="F10">
+        <v>9.9273320800025051E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>646948.58800000011</v>
+      </c>
+      <c r="D11">
+        <v>126328.47284772345</v>
+      </c>
+      <c r="E11">
+        <v>5.1854197463218711E-2</v>
+      </c>
+      <c r="F11">
+        <v>9.9434248994746868E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1665926.8079999995</v>
+      </c>
+      <c r="D12">
+        <v>184066.73734873536</v>
+      </c>
+      <c r="E12">
+        <v>9.5323738342314598E-2</v>
+      </c>
+      <c r="F12">
+        <v>1.3237367101276281E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1544196.5239999997</v>
+      </c>
+      <c r="D13">
+        <v>116715.17866666666</v>
+      </c>
+      <c r="E13">
+        <v>4.51093985918566E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7532258357421117E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A06D71C-2B86-EB48-85FD-54A340C7E5B0}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>91.706464681991335</v>
+      </c>
+      <c r="D2">
+        <v>0.28298816164686502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>89.135061830844222</v>
+      </c>
+      <c r="D3">
+        <v>0.19207804205708032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>87.798895764124168</v>
+      </c>
+      <c r="D4">
+        <v>0.29282962421735398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>84.829510402117066</v>
+      </c>
+      <c r="D5">
+        <v>4.8659849952064259E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>94.828390891100369</v>
+      </c>
+      <c r="D6">
+        <v>0.30888466340770077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>89.170616464379279</v>
+      </c>
+      <c r="D7">
+        <v>0.33748216586142676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>87.436467886799235</v>
+      </c>
+      <c r="D8">
+        <v>0.50428526194780987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>78.909663918532857</v>
+      </c>
+      <c r="D9">
+        <v>1.1118775714045055</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>93.586272564698788</v>
+      </c>
+      <c r="D10">
+        <v>0.45215710789145624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>88.99628406769132</v>
+      </c>
+      <c r="D11">
+        <v>0.58435394799197804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>87.077480780461556</v>
+      </c>
+      <c r="D12">
+        <v>0.69980860953902935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>80.187910340300675</v>
+      </c>
+      <c r="D13">
+        <v>0.72736303593831653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>101.69272901068801</v>
+      </c>
+      <c r="D14">
+        <v>0.97238769252775803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>88.504253816512872</v>
+      </c>
+      <c r="D15">
+        <v>1.1179276211029188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>87.056836154538004</v>
+      </c>
+      <c r="D16">
+        <v>0.39809487368559232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>84.416617883645642</v>
+      </c>
+      <c r="D17">
+        <v>1.2296268021546644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>